<commit_message>
fix training data issue
</commit_message>
<xml_diff>
--- a/EmeraldAI/Data/TrainingData/DE_Training.xlsx
+++ b/EmeraldAI/Data/TrainingData/DE_Training.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\EmeraldAI\EmeraldAI\Data\TrainingData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="315" windowWidth="25860" windowHeight="16665"/>
+    <workbookView xWindow="2040" yWindow="320" windowWidth="25860" windowHeight="16660"/>
   </bookViews>
   <sheets>
     <sheet name="Sentence" sheetId="1" r:id="rId1"/>
@@ -18,11 +13,11 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -454,9 +449,6 @@
     <t>Hey</t>
   </si>
   <si>
-    <t>Wie geht’s?</t>
-  </si>
-  <si>
     <t>Hilfe</t>
   </si>
   <si>
@@ -496,9 +488,6 @@
     <t>Bist du eine Mädchen</t>
   </si>
   <si>
-    <t>Wie geht’s dir?</t>
-  </si>
-  <si>
     <t>Was magst du?</t>
   </si>
   <si>
@@ -809,6 +798,12 @@
   </si>
   <si>
     <t>Höre für {number} Minuten weg.</t>
+  </si>
+  <si>
+    <t>Wie gehts dir?</t>
+  </si>
+  <si>
+    <t>Wie gehts?</t>
   </si>
 </sst>
 </file>
@@ -925,32 +920,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="53">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -979,217 +974,7 @@
     <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="66">
     <dxf>
       <fill>
         <patternFill>
@@ -1920,7 +1705,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1930,22 +1715,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
-      <selection activeCell="A191" sqref="A191"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" customWidth="1"/>
+    <col min="2" max="2" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1965,10 +1750,10 @@
         <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1979,7 +1764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1990,7 +1775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2001,7 +1786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2012,7 +1797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2023,7 +1808,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2034,7 +1819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2045,7 +1830,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2056,7 +1841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -2067,18 +1852,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2089,7 +1874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2100,7 +1885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -2114,7 +1899,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2125,7 +1910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -2142,7 +1927,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -2159,7 +1944,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -2173,7 +1958,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2187,7 +1972,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -2204,7 +1989,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2221,7 +2006,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -2238,7 +2023,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -2255,7 +2040,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -2272,7 +2057,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -2286,7 +2071,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -2297,7 +2082,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -2308,12 +2093,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C29" t="s">
         <v>34</v>
@@ -2325,7 +2110,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -2336,7 +2121,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -2347,7 +2132,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -2358,7 +2143,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -2369,7 +2154,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -2380,18 +2165,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -2402,7 +2187,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -2413,7 +2198,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -2427,7 +2212,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -2438,7 +2223,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -2449,7 +2234,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -2460,7 +2245,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -2471,7 +2256,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2482,7 +2267,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -2499,7 +2284,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -2510,7 +2295,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -2521,7 +2306,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -2532,7 +2317,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -2540,7 +2325,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -2551,10 +2336,10 @@
         <v>95</v>
       </c>
       <c r="F53" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2565,10 +2350,10 @@
         <v>96</v>
       </c>
       <c r="F54" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -2579,7 +2364,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -2590,7 +2375,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -2601,7 +2386,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -2612,7 +2397,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>5</v>
       </c>
@@ -2623,7 +2408,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -2634,7 +2419,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -2645,7 +2430,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -2659,10 +2444,10 @@
         <v>103</v>
       </c>
       <c r="F63" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -2676,10 +2461,10 @@
         <v>103</v>
       </c>
       <c r="F64" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -2693,32 +2478,32 @@
         <v>103</v>
       </c>
       <c r="F65" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>141</v>
+        <v>259</v>
       </c>
       <c r="E67" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>155</v>
+        <v>258</v>
       </c>
       <c r="E68" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>5</v>
       </c>
@@ -2729,7 +2514,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>5</v>
       </c>
@@ -2740,7 +2525,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -2751,7 +2536,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -2765,7 +2550,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -2779,7 +2564,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -2790,7 +2575,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>5</v>
       </c>
@@ -2801,18 +2586,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E77" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -2823,7 +2608,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -2834,7 +2619,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>8</v>
       </c>
@@ -2848,59 +2633,59 @@
         <v>120</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E82" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E83" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>5</v>
       </c>
       <c r="C84" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E84" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E85" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>8</v>
       </c>
       <c r="B86" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C86" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D86" t="s">
         <v>32</v>
@@ -2909,288 +2694,288 @@
         <v>122</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>5</v>
       </c>
       <c r="C88" t="s">
+        <v>141</v>
+      </c>
+      <c r="E88" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" t="s">
         <v>142</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E89" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" t="s">
+        <v>143</v>
+      </c>
+      <c r="E90" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" t="s">
+        <v>188</v>
+      </c>
+      <c r="D91" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" t="s">
-        <v>143</v>
-      </c>
-      <c r="E89" t="s">
+    <row r="92" spans="1:6">
+      <c r="A92" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" t="s">
+        <v>190</v>
+      </c>
+      <c r="D92" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" t="s">
+    <row r="93" spans="1:6">
+      <c r="A93" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" t="s">
+        <v>191</v>
+      </c>
+      <c r="D93" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" t="s">
         <v>144</v>
       </c>
-      <c r="E90" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>8</v>
-      </c>
-      <c r="C91" t="s">
-        <v>190</v>
-      </c>
-      <c r="D91" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>8</v>
-      </c>
-      <c r="C92" t="s">
-        <v>192</v>
-      </c>
-      <c r="D92" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>8</v>
-      </c>
-      <c r="C93" t="s">
-        <v>193</v>
-      </c>
-      <c r="D93" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>5</v>
-      </c>
-      <c r="C95" t="s">
+      <c r="E95" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" t="s">
+        <v>213</v>
+      </c>
+      <c r="D96" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" t="s">
+        <v>214</v>
+      </c>
+      <c r="E98" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" t="s">
+        <v>215</v>
+      </c>
+      <c r="E99" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" t="s">
+        <v>216</v>
+      </c>
+      <c r="E100" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" t="s">
+        <v>217</v>
+      </c>
+      <c r="E101" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" t="s">
+        <v>218</v>
+      </c>
+      <c r="D102" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>8</v>
+      </c>
+      <c r="C103" t="s">
+        <v>219</v>
+      </c>
+      <c r="D103" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" t="s">
         <v>145</v>
       </c>
-      <c r="E95" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>8</v>
-      </c>
-      <c r="C96" t="s">
-        <v>215</v>
-      </c>
-      <c r="D96" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" t="s">
-        <v>216</v>
-      </c>
-      <c r="E98" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99" t="s">
-        <v>217</v>
-      </c>
-      <c r="E99" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" t="s">
-        <v>218</v>
-      </c>
-      <c r="E100" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" t="s">
-        <v>219</v>
-      </c>
-      <c r="E101" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>8</v>
-      </c>
-      <c r="C102" t="s">
+      <c r="E105" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" t="s">
+        <v>146</v>
+      </c>
+      <c r="E106" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" t="s">
+        <v>152</v>
+      </c>
+      <c r="E107" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>5</v>
+      </c>
+      <c r="C108" t="s">
+        <v>153</v>
+      </c>
+      <c r="E108" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" t="s">
+        <v>147</v>
+      </c>
+      <c r="E109" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" t="s">
         <v>220</v>
       </c>
-      <c r="D102" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>8</v>
-      </c>
-      <c r="C103" t="s">
+      <c r="E110" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111" t="s">
         <v>221</v>
       </c>
-      <c r="D103" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105" t="s">
-        <v>146</v>
-      </c>
-      <c r="E105" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>5</v>
-      </c>
-      <c r="C106" t="s">
-        <v>147</v>
-      </c>
-      <c r="E106" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>5</v>
-      </c>
-      <c r="C107" t="s">
-        <v>153</v>
-      </c>
-      <c r="E107" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>5</v>
-      </c>
-      <c r="C108" t="s">
-        <v>154</v>
-      </c>
-      <c r="E108" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>5</v>
-      </c>
-      <c r="C109" t="s">
+      <c r="C111" t="s">
+        <v>222</v>
+      </c>
+      <c r="D111" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" t="s">
+        <v>8</v>
+      </c>
+      <c r="B112" t="s">
+        <v>223</v>
+      </c>
+      <c r="C112" t="s">
+        <v>224</v>
+      </c>
+      <c r="D112" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" t="s">
+        <v>8</v>
+      </c>
+      <c r="C113" t="s">
+        <v>225</v>
+      </c>
+      <c r="D113" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115" t="s">
         <v>148</v>
       </c>
-      <c r="E109" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" t="s">
-        <v>222</v>
-      </c>
-      <c r="E110" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>8</v>
-      </c>
-      <c r="B111" t="s">
-        <v>223</v>
-      </c>
-      <c r="C111" t="s">
-        <v>224</v>
-      </c>
-      <c r="D111" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>8</v>
-      </c>
-      <c r="B112" t="s">
-        <v>225</v>
-      </c>
-      <c r="C112" t="s">
-        <v>226</v>
-      </c>
-      <c r="D112" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>8</v>
-      </c>
-      <c r="C113" t="s">
-        <v>227</v>
-      </c>
-      <c r="D113" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>5</v>
-      </c>
-      <c r="C115" t="s">
+      <c r="E115" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C116" t="s">
         <v>149</v>
       </c>
-      <c r="E115" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>5</v>
-      </c>
-      <c r="C116" t="s">
-        <v>150</v>
-      </c>
       <c r="E116" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
         <v>8</v>
       </c>
@@ -3198,462 +2983,462 @@
         <v>139</v>
       </c>
       <c r="D117" t="s">
+        <v>156</v>
+      </c>
+      <c r="F117" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" t="s">
+        <v>5</v>
+      </c>
+      <c r="C119" t="s">
+        <v>182</v>
+      </c>
+      <c r="E119" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" t="s">
+        <v>5</v>
+      </c>
+      <c r="C120" t="s">
+        <v>181</v>
+      </c>
+      <c r="E120" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" t="s">
+        <v>5</v>
+      </c>
+      <c r="C121" t="s">
+        <v>183</v>
+      </c>
+      <c r="E121" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" t="s">
+        <v>8</v>
+      </c>
+      <c r="C122" t="s">
+        <v>184</v>
+      </c>
+      <c r="D122" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" t="s">
+        <v>8</v>
+      </c>
+      <c r="C123" t="s">
+        <v>185</v>
+      </c>
+      <c r="D123" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" t="s">
+        <v>5</v>
+      </c>
+      <c r="C125" t="s">
+        <v>177</v>
+      </c>
+      <c r="E125" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126" t="s">
+        <v>178</v>
+      </c>
+      <c r="E126" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" t="s">
+        <v>8</v>
+      </c>
+      <c r="C127" t="s">
+        <v>179</v>
+      </c>
+      <c r="D127" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" t="s">
+        <v>8</v>
+      </c>
+      <c r="C128" t="s">
+        <v>180</v>
+      </c>
+      <c r="D128" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" t="s">
+        <v>5</v>
+      </c>
+      <c r="C130" t="s">
+        <v>168</v>
+      </c>
+      <c r="E130" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" t="s">
+        <v>5</v>
+      </c>
+      <c r="C131" t="s">
+        <v>169</v>
+      </c>
+      <c r="E131" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" t="s">
+        <v>8</v>
+      </c>
+      <c r="C132" t="s">
+        <v>172</v>
+      </c>
+      <c r="D132" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" t="s">
+        <v>8</v>
+      </c>
+      <c r="C133" t="s">
+        <v>174</v>
+      </c>
+      <c r="D133" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" t="s">
+        <v>5</v>
+      </c>
+      <c r="C135" t="s">
+        <v>170</v>
+      </c>
+      <c r="E135" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" t="s">
+        <v>5</v>
+      </c>
+      <c r="C136" t="s">
+        <v>171</v>
+      </c>
+      <c r="E136" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" t="s">
+        <v>8</v>
+      </c>
+      <c r="C137" t="s">
+        <v>175</v>
+      </c>
+      <c r="D137" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" t="s">
+        <v>8</v>
+      </c>
+      <c r="C138" t="s">
+        <v>176</v>
+      </c>
+      <c r="D138" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" t="s">
+        <v>5</v>
+      </c>
+      <c r="C140" t="s">
         <v>158</v>
       </c>
-      <c r="F117" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>5</v>
-      </c>
-      <c r="C119" t="s">
-        <v>184</v>
-      </c>
-      <c r="E119" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>5</v>
-      </c>
-      <c r="C120" t="s">
-        <v>183</v>
-      </c>
-      <c r="E120" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>5</v>
-      </c>
-      <c r="C121" t="s">
-        <v>185</v>
-      </c>
-      <c r="E121" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>8</v>
-      </c>
-      <c r="C122" t="s">
-        <v>186</v>
-      </c>
-      <c r="D122" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>8</v>
-      </c>
-      <c r="C123" t="s">
-        <v>187</v>
-      </c>
-      <c r="D123" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>5</v>
-      </c>
-      <c r="C125" t="s">
-        <v>179</v>
-      </c>
-      <c r="E125" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>5</v>
-      </c>
-      <c r="C126" t="s">
-        <v>180</v>
-      </c>
-      <c r="E126" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>8</v>
-      </c>
-      <c r="C127" t="s">
-        <v>181</v>
-      </c>
-      <c r="D127" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>8</v>
-      </c>
-      <c r="C128" t="s">
-        <v>182</v>
-      </c>
-      <c r="D128" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>5</v>
-      </c>
-      <c r="C130" t="s">
-        <v>170</v>
-      </c>
-      <c r="E130" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>5</v>
-      </c>
-      <c r="C131" t="s">
-        <v>171</v>
-      </c>
-      <c r="E131" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>8</v>
-      </c>
-      <c r="C132" t="s">
-        <v>174</v>
-      </c>
-      <c r="D132" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>8</v>
-      </c>
-      <c r="C133" t="s">
-        <v>176</v>
-      </c>
-      <c r="D133" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>5</v>
-      </c>
-      <c r="C135" t="s">
-        <v>172</v>
-      </c>
-      <c r="E135" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>5</v>
-      </c>
-      <c r="C136" t="s">
+      <c r="E140" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" t="s">
+        <v>5</v>
+      </c>
+      <c r="C141" t="s">
+        <v>159</v>
+      </c>
+      <c r="E141" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" t="s">
+        <v>5</v>
+      </c>
+      <c r="C142" t="s">
+        <v>160</v>
+      </c>
+      <c r="E142" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" t="s">
+        <v>8</v>
+      </c>
+      <c r="C143" t="s">
+        <v>165</v>
+      </c>
+      <c r="D143" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" t="s">
+        <v>8</v>
+      </c>
+      <c r="C144" t="s">
+        <v>166</v>
+      </c>
+      <c r="D144" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" t="s">
+        <v>5</v>
+      </c>
+      <c r="C146" t="s">
+        <v>161</v>
+      </c>
+      <c r="E146" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147" t="s">
+        <v>162</v>
+      </c>
+      <c r="E147" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" t="s">
+        <v>5</v>
+      </c>
+      <c r="C148" t="s">
+        <v>163</v>
+      </c>
+      <c r="E148" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
+      <c r="A149" t="s">
+        <v>8</v>
+      </c>
+      <c r="C149" t="s">
+        <v>164</v>
+      </c>
+      <c r="D149" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" t="s">
+        <v>8</v>
+      </c>
+      <c r="C150" t="s">
+        <v>167</v>
+      </c>
+      <c r="D150" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
+      <c r="A152" t="s">
+        <v>5</v>
+      </c>
+      <c r="C152" t="s">
+        <v>154</v>
+      </c>
+      <c r="E152" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" t="s">
+        <v>5</v>
+      </c>
+      <c r="C153" t="s">
+        <v>155</v>
+      </c>
+      <c r="E153" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
+      <c r="A154" t="s">
+        <v>8</v>
+      </c>
+      <c r="C154" t="s">
+        <v>157</v>
+      </c>
+      <c r="D154" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="A155" t="s">
+        <v>8</v>
+      </c>
+      <c r="C155" t="s">
         <v>173</v>
       </c>
-      <c r="E136" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>8</v>
-      </c>
-      <c r="C137" t="s">
-        <v>177</v>
-      </c>
-      <c r="D137" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>8</v>
-      </c>
-      <c r="C138" t="s">
-        <v>178</v>
-      </c>
-      <c r="D138" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>5</v>
-      </c>
-      <c r="C140" t="s">
-        <v>160</v>
-      </c>
-      <c r="E140" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>5</v>
-      </c>
-      <c r="C141" t="s">
-        <v>161</v>
-      </c>
-      <c r="E141" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>5</v>
-      </c>
-      <c r="C142" t="s">
-        <v>162</v>
-      </c>
-      <c r="E142" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>8</v>
-      </c>
-      <c r="C143" t="s">
-        <v>167</v>
-      </c>
-      <c r="D143" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>8</v>
-      </c>
-      <c r="C144" t="s">
-        <v>168</v>
-      </c>
-      <c r="D144" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>5</v>
-      </c>
-      <c r="C146" t="s">
-        <v>163</v>
-      </c>
-      <c r="E146" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>5</v>
-      </c>
-      <c r="C147" t="s">
-        <v>164</v>
-      </c>
-      <c r="E147" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>5</v>
-      </c>
-      <c r="C148" t="s">
-        <v>165</v>
-      </c>
-      <c r="E148" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>8</v>
-      </c>
-      <c r="C149" t="s">
-        <v>166</v>
-      </c>
-      <c r="D149" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>8</v>
-      </c>
-      <c r="C150" t="s">
-        <v>169</v>
-      </c>
-      <c r="D150" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>5</v>
-      </c>
-      <c r="C152" t="s">
-        <v>156</v>
-      </c>
-      <c r="E152" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>5</v>
-      </c>
-      <c r="C153" t="s">
-        <v>157</v>
-      </c>
-      <c r="E153" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>8</v>
-      </c>
-      <c r="C154" t="s">
-        <v>159</v>
-      </c>
-      <c r="D154" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>8</v>
-      </c>
-      <c r="C155" t="s">
-        <v>175</v>
-      </c>
       <c r="D155" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
       <c r="A157" t="s">
         <v>5</v>
       </c>
       <c r="C157" t="s">
+        <v>206</v>
+      </c>
+      <c r="E157" t="s">
         <v>208</v>
       </c>
-      <c r="E157" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="158" spans="1:7">
       <c r="A158" t="s">
         <v>8</v>
       </c>
       <c r="C158" t="s">
+        <v>205</v>
+      </c>
+      <c r="D158" t="s">
+        <v>208</v>
+      </c>
+      <c r="G158" t="s">
         <v>207</v>
       </c>
-      <c r="D158" t="s">
-        <v>210</v>
-      </c>
-      <c r="G158" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="160" spans="1:7">
       <c r="A160" t="s">
         <v>5</v>
       </c>
       <c r="C160" t="s">
+        <v>226</v>
+      </c>
+      <c r="E160" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
+      <c r="A161" t="s">
+        <v>8</v>
+      </c>
+      <c r="C161" t="s">
+        <v>227</v>
+      </c>
+      <c r="D161" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7">
+      <c r="A162" t="s">
+        <v>8</v>
+      </c>
+      <c r="C162" t="s">
         <v>228</v>
       </c>
-      <c r="E160" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>8</v>
-      </c>
-      <c r="C161" t="s">
-        <v>229</v>
-      </c>
-      <c r="D161" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>8</v>
-      </c>
-      <c r="C162" t="s">
-        <v>230</v>
-      </c>
       <c r="D162" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7">
       <c r="A164" t="s">
         <v>5</v>
       </c>
       <c r="C164" t="s">
+        <v>192</v>
+      </c>
+      <c r="E164" t="s">
         <v>194</v>
       </c>
-      <c r="E164" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="165" spans="1:7">
       <c r="A165" t="s">
         <v>8</v>
       </c>
       <c r="C165" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D165" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G165" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7">
       <c r="A166" t="s">
         <v>8</v>
       </c>
       <c r="C166" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D166" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G166" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7">
       <c r="A168" t="s">
         <v>5</v>
       </c>
       <c r="C168" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E168" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7">
       <c r="A169" t="s">
         <v>8</v>
       </c>
@@ -3661,46 +3446,46 @@
         <v>73</v>
       </c>
       <c r="C169" t="s">
+        <v>195</v>
+      </c>
+      <c r="D169" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7">
+      <c r="A170" t="s">
+        <v>8</v>
+      </c>
+      <c r="C170" t="s">
+        <v>196</v>
+      </c>
+      <c r="D170" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7">
+      <c r="A171" t="s">
+        <v>8</v>
+      </c>
+      <c r="C171" t="s">
         <v>197</v>
       </c>
-      <c r="D169" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>8</v>
-      </c>
-      <c r="C170" t="s">
-        <v>198</v>
-      </c>
-      <c r="D170" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>8</v>
-      </c>
-      <c r="C171" t="s">
-        <v>199</v>
-      </c>
       <c r="D171" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7">
       <c r="A173" t="s">
         <v>5</v>
       </c>
       <c r="C173" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E173" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7">
       <c r="A174" t="s">
         <v>8</v>
       </c>
@@ -3708,13 +3493,13 @@
         <v>73</v>
       </c>
       <c r="C174" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D174" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7">
       <c r="A175" t="s">
         <v>8</v>
       </c>
@@ -3722,393 +3507,392 @@
         <v>73</v>
       </c>
       <c r="C175" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D175" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7">
       <c r="A176" t="s">
         <v>8</v>
       </c>
       <c r="C176" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D176" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7">
       <c r="A178" t="s">
         <v>5</v>
       </c>
       <c r="C178" t="s">
+        <v>245</v>
+      </c>
+      <c r="E178" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7">
+      <c r="A179" t="s">
+        <v>5</v>
+      </c>
+      <c r="C179" t="s">
+        <v>246</v>
+      </c>
+      <c r="E179" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7">
+      <c r="A180" t="s">
+        <v>5</v>
+      </c>
+      <c r="C180" t="s">
         <v>247</v>
       </c>
-      <c r="E178" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>5</v>
-      </c>
-      <c r="C179" t="s">
-        <v>248</v>
-      </c>
-      <c r="E179" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>5</v>
-      </c>
-      <c r="C180" t="s">
-        <v>249</v>
-      </c>
       <c r="E180" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7">
       <c r="A181" t="s">
         <v>8</v>
       </c>
       <c r="D181" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F181" t="s">
+        <v>250</v>
+      </c>
+      <c r="G181" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7">
+      <c r="A183" t="s">
+        <v>5</v>
+      </c>
+      <c r="C183" t="s">
+        <v>251</v>
+      </c>
+      <c r="E183" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7">
+      <c r="A184" t="s">
+        <v>5</v>
+      </c>
+      <c r="C184" t="s">
         <v>252</v>
       </c>
-      <c r="G181" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>5</v>
-      </c>
-      <c r="C183" t="s">
+      <c r="E184" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7">
+      <c r="A185" t="s">
+        <v>8</v>
+      </c>
+      <c r="D185" t="s">
+        <v>194</v>
+      </c>
+      <c r="F185" t="s">
         <v>253</v>
       </c>
-      <c r="E183" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>5</v>
-      </c>
-      <c r="C184" t="s">
+      <c r="G185" t="s">
         <v>254</v>
       </c>
-      <c r="E184" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>8</v>
-      </c>
-      <c r="D185" t="s">
-        <v>196</v>
-      </c>
-      <c r="F185" t="s">
+    </row>
+    <row r="187" spans="1:7">
+      <c r="A187" t="s">
+        <v>5</v>
+      </c>
+      <c r="C187" t="s">
         <v>255</v>
       </c>
-      <c r="G185" t="s">
+      <c r="E187" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7">
+      <c r="A188" t="s">
+        <v>5</v>
+      </c>
+      <c r="C188" t="s">
+        <v>257</v>
+      </c>
+      <c r="E188" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7">
+      <c r="A189" t="s">
+        <v>8</v>
+      </c>
+      <c r="D189" t="s">
+        <v>194</v>
+      </c>
+      <c r="F189" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>5</v>
-      </c>
-      <c r="C187" t="s">
-        <v>257</v>
-      </c>
-      <c r="E187" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>5</v>
-      </c>
-      <c r="C188" t="s">
-        <v>259</v>
-      </c>
-      <c r="E188" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>8</v>
-      </c>
-      <c r="D189" t="s">
-        <v>196</v>
-      </c>
-      <c r="F189" t="s">
-        <v>258</v>
-      </c>
       <c r="G189" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A115:G158 A79:G81 A88:G94 A1:G77 A163:G187 A189:G1048576 A188:C188 E188:G188">
-    <cfRule type="expression" dxfId="67" priority="121">
+    <cfRule type="expression" dxfId="65" priority="121">
       <formula>$A1="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="122">
+    <cfRule type="expression" dxfId="64" priority="122">
       <formula>$A1="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88:G93">
-    <cfRule type="expression" dxfId="65" priority="59">
+    <cfRule type="expression" dxfId="63" priority="59">
       <formula>$A88="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="60">
+    <cfRule type="expression" dxfId="62" priority="60">
       <formula>$A88="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B157">
-    <cfRule type="expression" dxfId="63" priority="57">
+    <cfRule type="expression" dxfId="61" priority="57">
       <formula>$A157="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="58">
+    <cfRule type="expression" dxfId="60" priority="58">
       <formula>$A157="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A114:G114 A97:G97 A105:D110 F105:G110 A112:C113 E112:G113 A104:G104 A102:C103 E102:G103 A98:D101 F98:G101 A95:D95 F95:G95 A96:C96 E96:G96">
-    <cfRule type="expression" dxfId="61" priority="53">
+    <cfRule type="expression" dxfId="59" priority="53">
       <formula>$A95="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="54">
+    <cfRule type="expression" dxfId="58" priority="54">
       <formula>$A95="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A114:G114 A97:G97 A105:D110 F105:G110 A112:C113 E112:G113 A104:G104 A102:C103 E102:G103 A98:D101 F98:G101 A95:D95 F95:G95 A96:C96 E96:G96">
-    <cfRule type="expression" dxfId="59" priority="55">
+    <cfRule type="expression" dxfId="57" priority="55">
       <formula>$A95="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="56">
+    <cfRule type="expression" dxfId="56" priority="56">
       <formula>$A95="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A111:C111 E111:G111">
-    <cfRule type="expression" dxfId="57" priority="49">
+    <cfRule type="expression" dxfId="55" priority="49">
       <formula>$A111="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="50">
+    <cfRule type="expression" dxfId="54" priority="50">
       <formula>$A111="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A111:C111 E111:G111">
-    <cfRule type="expression" dxfId="55" priority="51">
+    <cfRule type="expression" dxfId="53" priority="51">
       <formula>$A111="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="52">
+    <cfRule type="expression" dxfId="52" priority="52">
       <formula>$A111="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A159:G162">
-    <cfRule type="expression" dxfId="53" priority="47">
+    <cfRule type="expression" dxfId="51" priority="47">
       <formula>$A159="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="48">
+    <cfRule type="expression" dxfId="50" priority="48">
       <formula>$A159="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E105">
-    <cfRule type="expression" dxfId="51" priority="45">
+    <cfRule type="expression" dxfId="49" priority="45">
       <formula>$A105="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="46">
+    <cfRule type="expression" dxfId="48" priority="46">
       <formula>$A105="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106">
-    <cfRule type="expression" dxfId="49" priority="43">
+    <cfRule type="expression" dxfId="47" priority="43">
       <formula>$A106="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="44">
+    <cfRule type="expression" dxfId="46" priority="44">
       <formula>$A106="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107">
-    <cfRule type="expression" dxfId="47" priority="41">
+    <cfRule type="expression" dxfId="45" priority="41">
       <formula>$A107="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="42">
+    <cfRule type="expression" dxfId="44" priority="42">
       <formula>$A107="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E108">
-    <cfRule type="expression" dxfId="45" priority="39">
+    <cfRule type="expression" dxfId="43" priority="39">
       <formula>$A108="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="40">
+    <cfRule type="expression" dxfId="42" priority="40">
       <formula>$A108="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109">
-    <cfRule type="expression" dxfId="43" priority="37">
+    <cfRule type="expression" dxfId="41" priority="37">
       <formula>$A109="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="38">
+    <cfRule type="expression" dxfId="40" priority="38">
       <formula>$A109="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E110">
-    <cfRule type="expression" dxfId="41" priority="35">
+    <cfRule type="expression" dxfId="39" priority="35">
       <formula>$A110="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="36">
+    <cfRule type="expression" dxfId="38" priority="36">
       <formula>$A110="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D111">
-    <cfRule type="expression" dxfId="39" priority="33">
+    <cfRule type="expression" dxfId="37" priority="33">
       <formula>$A111="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="34">
+    <cfRule type="expression" dxfId="36" priority="34">
       <formula>$A111="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D112">
-    <cfRule type="expression" dxfId="37" priority="31">
+    <cfRule type="expression" dxfId="35" priority="31">
       <formula>$A112="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="32">
+    <cfRule type="expression" dxfId="34" priority="32">
       <formula>$A112="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D113">
-    <cfRule type="expression" dxfId="35" priority="29">
+    <cfRule type="expression" dxfId="33" priority="29">
       <formula>$A113="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="30">
+    <cfRule type="expression" dxfId="32" priority="30">
       <formula>$A113="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="expression" dxfId="33" priority="27">
+    <cfRule type="expression" dxfId="31" priority="27">
       <formula>$A103="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="28">
+    <cfRule type="expression" dxfId="30" priority="28">
       <formula>$A103="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D102">
-    <cfRule type="expression" dxfId="31" priority="25">
+    <cfRule type="expression" dxfId="29" priority="25">
       <formula>$A102="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="26">
+    <cfRule type="expression" dxfId="28" priority="26">
       <formula>$A102="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E101">
-    <cfRule type="expression" dxfId="29" priority="23">
+    <cfRule type="expression" dxfId="27" priority="23">
       <formula>$A101="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="24">
+    <cfRule type="expression" dxfId="26" priority="24">
       <formula>$A101="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E100">
-    <cfRule type="expression" dxfId="27" priority="21">
+    <cfRule type="expression" dxfId="25" priority="21">
       <formula>$A100="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="22">
+    <cfRule type="expression" dxfId="24" priority="22">
       <formula>$A100="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E99">
-    <cfRule type="expression" dxfId="25" priority="19">
+    <cfRule type="expression" dxfId="23" priority="19">
       <formula>$A99="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="20">
+    <cfRule type="expression" dxfId="22" priority="20">
       <formula>$A99="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E98">
-    <cfRule type="expression" dxfId="23" priority="17">
+    <cfRule type="expression" dxfId="21" priority="17">
       <formula>$A98="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="18">
+    <cfRule type="expression" dxfId="20" priority="18">
       <formula>$A98="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E95">
-    <cfRule type="expression" dxfId="21" priority="15">
+    <cfRule type="expression" dxfId="19" priority="15">
       <formula>$A95="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="16">
+    <cfRule type="expression" dxfId="18" priority="16">
       <formula>$A95="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D96">
-    <cfRule type="expression" dxfId="19" priority="13">
+    <cfRule type="expression" dxfId="17" priority="13">
       <formula>$A96="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="14">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>$A96="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78:G78">
-    <cfRule type="expression" dxfId="17" priority="11">
+    <cfRule type="expression" dxfId="15" priority="11">
       <formula>$A78="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="12">
+    <cfRule type="expression" dxfId="14" priority="12">
       <formula>$A78="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83:G83 A86:G87">
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="13" priority="9">
       <formula>$A83="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="10">
+    <cfRule type="expression" dxfId="12" priority="10">
       <formula>$A83="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:G82">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="11" priority="7">
       <formula>$A82="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="10" priority="8">
       <formula>$A82="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:G85">
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$A85="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>$A85="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84:G84">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>$A84="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>$A84="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D188">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$A188="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$A188="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4125,85 +3909,90 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="41.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>120</v>
       </c>
       <c r="B2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D2" t="s">
         <v>211</v>
       </c>
-      <c r="C2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$A1="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A1="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4215,21 +4004,21 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>76</v>
       </c>
@@ -4237,7 +4026,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="B4" t="s">
         <v>52</v>
       </c>
@@ -4245,27 +4034,27 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="C5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="C6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="C7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="B10" t="s">
         <v>58</v>
       </c>
@@ -4279,7 +4068,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="B11" t="s">
         <v>59</v>
       </c>
@@ -4293,7 +4082,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="B12" t="s">
         <v>60</v>
       </c>
@@ -4307,7 +4096,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="B13" t="s">
         <v>61</v>
       </c>
@@ -4321,7 +4110,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="B14" t="s">
         <v>62</v>
       </c>
@@ -4329,12 +4118,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="B17" t="s">
         <v>69</v>
       </c>
@@ -4342,7 +4131,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="B18" t="s">
         <v>71</v>
       </c>
@@ -4350,7 +4139,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="B19" t="s">
         <v>85</v>
       </c>
@@ -4358,7 +4147,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="B20" t="s">
         <v>110</v>
       </c>
@@ -4366,7 +4155,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="B21" t="s">
         <v>109</v>
       </c>
@@ -4374,12 +4163,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="B24" t="s">
         <v>120</v>
       </c>
@@ -4387,7 +4176,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="B25" t="s">
         <v>122</v>
       </c>
@@ -4395,7 +4184,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="B26" t="s">
         <v>124</v>
       </c>
@@ -4403,7 +4192,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="B27" t="s">
         <v>126</v>
       </c>
@@ -4411,7 +4200,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="B28" t="s">
         <v>128</v>
       </c>
@@ -4419,26 +4208,26 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>120</v>
       </c>
       <c r="B35" t="s">
+        <v>209</v>
+      </c>
+      <c r="C35" t="s">
+        <v>210</v>
+      </c>
+      <c r="D35" t="s">
         <v>211</v>
-      </c>
-      <c r="C35" t="s">
-        <v>212</v>
-      </c>
-      <c r="D35" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F28">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$A1="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$A1="Q"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update base training File
</commit_message>
<xml_diff>
--- a/EmeraldAI/Data/TrainingData/DE_Training.xlsx
+++ b/EmeraldAI/Data/TrainingData/DE_Training.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="268">
   <si>
     <t>Requirement</t>
   </si>
@@ -591,9 +591,6 @@
     <t>TRIGGER_FACEAPP_OFF</t>
   </si>
   <si>
-    <t>TRIGGER</t>
-  </si>
-  <si>
     <t>Hey, wer hat das List aus gemacht?</t>
   </si>
   <si>
@@ -814,6 +811,24 @@
   </si>
   <si>
     <t>WordType:UserLastname</t>
+  </si>
+  <si>
+    <t>TRIGGER|FACEAPP_ON</t>
+  </si>
+  <si>
+    <t>TRIGGER|FACEAPP_OFF</t>
+  </si>
+  <si>
+    <t>TRIGGER|Intruder</t>
+  </si>
+  <si>
+    <t>TRIGGER|Mute</t>
+  </si>
+  <si>
+    <t>TRIGGER|Unmute</t>
+  </si>
+  <si>
+    <t>TRIGGER|Deaf</t>
   </si>
 </sst>
 </file>
@@ -870,8 +885,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -937,7 +968,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="77">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -968,6 +999,14 @@
     <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -998,9 +1037,241 @@
     <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="98">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1741,8 +2012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="D189" sqref="D189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1776,7 +2047,7 @@
         <v>116</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2124,7 +2395,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C29" t="s">
         <v>34</v>
@@ -2362,7 +2633,7 @@
         <v>95</v>
       </c>
       <c r="F53" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2376,7 +2647,7 @@
         <v>96</v>
       </c>
       <c r="F54" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2461,7 +2732,7 @@
         <v>8</v>
       </c>
       <c r="B63" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C63" t="s">
         <v>97</v>
@@ -2470,7 +2741,7 @@
         <v>103</v>
       </c>
       <c r="F63" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2478,7 +2749,7 @@
         <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C64" t="s">
         <v>99</v>
@@ -2487,7 +2758,7 @@
         <v>103</v>
       </c>
       <c r="F64" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2495,7 +2766,7 @@
         <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C65" t="s">
         <v>98</v>
@@ -2504,7 +2775,7 @@
         <v>103</v>
       </c>
       <c r="F65" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2512,7 +2783,7 @@
         <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E67" t="s">
         <v>21</v>
@@ -2523,7 +2794,7 @@
         <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E68" t="s">
         <v>21</v>
@@ -2567,10 +2838,10 @@
         <v>8</v>
       </c>
       <c r="B72" t="s">
+        <v>253</v>
+      </c>
+      <c r="C72" t="s">
         <v>254</v>
-      </c>
-      <c r="C72" t="s">
-        <v>255</v>
       </c>
       <c r="D72" t="s">
         <v>21</v>
@@ -2584,7 +2855,7 @@
         <v>115</v>
       </c>
       <c r="C73" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D73" t="s">
         <v>21</v>
@@ -2617,7 +2888,7 @@
         <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E77" t="s">
         <v>32</v>
@@ -2664,7 +2935,7 @@
         <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E82" t="s">
         <v>32</v>
@@ -2675,7 +2946,7 @@
         <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E83" t="s">
         <v>32</v>
@@ -2686,7 +2957,7 @@
         <v>5</v>
       </c>
       <c r="C84" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E84" t="s">
         <v>32</v>
@@ -2697,7 +2968,7 @@
         <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E85" t="s">
         <v>32</v>
@@ -2708,10 +2979,10 @@
         <v>8</v>
       </c>
       <c r="B86" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C86" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D86" t="s">
         <v>32</v>
@@ -2802,7 +3073,7 @@
         <v>8</v>
       </c>
       <c r="C96" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D96" t="s">
         <v>150</v>
@@ -2813,7 +3084,7 @@
         <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E98" t="s">
         <v>150</v>
@@ -2824,7 +3095,7 @@
         <v>5</v>
       </c>
       <c r="C99" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E99" t="s">
         <v>150</v>
@@ -2835,7 +3106,7 @@
         <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E100" t="s">
         <v>150</v>
@@ -2846,7 +3117,7 @@
         <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E101" t="s">
         <v>150</v>
@@ -2857,7 +3128,7 @@
         <v>8</v>
       </c>
       <c r="C102" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D102" t="s">
         <v>150</v>
@@ -2868,7 +3139,7 @@
         <v>8</v>
       </c>
       <c r="C103" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D103" t="s">
         <v>150</v>
@@ -2934,7 +3205,7 @@
         <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E110" t="s">
         <v>150</v>
@@ -2945,10 +3216,10 @@
         <v>8</v>
       </c>
       <c r="B111" t="s">
+        <v>214</v>
+      </c>
+      <c r="C111" t="s">
         <v>215</v>
-      </c>
-      <c r="C111" t="s">
-        <v>216</v>
       </c>
       <c r="D111" t="s">
         <v>150</v>
@@ -2959,10 +3230,10 @@
         <v>8</v>
       </c>
       <c r="B112" t="s">
+        <v>216</v>
+      </c>
+      <c r="C112" t="s">
         <v>217</v>
-      </c>
-      <c r="C112" t="s">
-        <v>218</v>
       </c>
       <c r="D112" t="s">
         <v>150</v>
@@ -2973,7 +3244,7 @@
         <v>8</v>
       </c>
       <c r="C113" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D113" t="s">
         <v>150</v>
@@ -3361,10 +3632,10 @@
         <v>5</v>
       </c>
       <c r="C157" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E157" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="158" spans="1:7">
@@ -3372,13 +3643,13 @@
         <v>8</v>
       </c>
       <c r="C158" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D158" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G158" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="160" spans="1:7">
@@ -3386,7 +3657,7 @@
         <v>5</v>
       </c>
       <c r="C160" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E160" t="s">
         <v>150</v>
@@ -3397,7 +3668,7 @@
         <v>8</v>
       </c>
       <c r="C161" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D161" t="s">
         <v>150</v>
@@ -3408,7 +3679,7 @@
         <v>8</v>
       </c>
       <c r="C162" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D162" t="s">
         <v>150</v>
@@ -3422,7 +3693,7 @@
         <v>186</v>
       </c>
       <c r="E164" t="s">
-        <v>188</v>
+        <v>262</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -3430,13 +3701,13 @@
         <v>8</v>
       </c>
       <c r="C165" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D165" t="s">
-        <v>188</v>
+        <v>262</v>
       </c>
       <c r="G165" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -3444,13 +3715,13 @@
         <v>8</v>
       </c>
       <c r="C166" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D166" t="s">
-        <v>188</v>
+        <v>262</v>
       </c>
       <c r="G166" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -3461,7 +3732,7 @@
         <v>187</v>
       </c>
       <c r="E168" t="s">
-        <v>188</v>
+        <v>263</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -3472,10 +3743,10 @@
         <v>73</v>
       </c>
       <c r="C169" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D169" t="s">
-        <v>188</v>
+        <v>263</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -3483,10 +3754,10 @@
         <v>8</v>
       </c>
       <c r="C170" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D170" t="s">
-        <v>188</v>
+        <v>263</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -3494,10 +3765,10 @@
         <v>8</v>
       </c>
       <c r="C171" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D171" t="s">
-        <v>188</v>
+        <v>263</v>
       </c>
     </row>
     <row r="173" spans="1:7">
@@ -3505,10 +3776,10 @@
         <v>5</v>
       </c>
       <c r="C173" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E173" t="s">
-        <v>188</v>
+        <v>264</v>
       </c>
     </row>
     <row r="174" spans="1:7">
@@ -3519,10 +3790,10 @@
         <v>73</v>
       </c>
       <c r="C174" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D174" t="s">
-        <v>188</v>
+        <v>264</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -3533,10 +3804,10 @@
         <v>73</v>
       </c>
       <c r="C175" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D175" t="s">
-        <v>188</v>
+        <v>264</v>
       </c>
     </row>
     <row r="176" spans="1:7">
@@ -3544,10 +3815,10 @@
         <v>8</v>
       </c>
       <c r="C176" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D176" t="s">
-        <v>188</v>
+        <v>264</v>
       </c>
     </row>
     <row r="178" spans="1:7">
@@ -3555,10 +3826,10 @@
         <v>5</v>
       </c>
       <c r="C178" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E178" t="s">
-        <v>188</v>
+        <v>265</v>
       </c>
     </row>
     <row r="179" spans="1:7">
@@ -3566,10 +3837,10 @@
         <v>5</v>
       </c>
       <c r="C179" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E179" t="s">
-        <v>188</v>
+        <v>265</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -3577,10 +3848,10 @@
         <v>5</v>
       </c>
       <c r="C180" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E180" t="s">
-        <v>188</v>
+        <v>265</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -3588,13 +3859,13 @@
         <v>8</v>
       </c>
       <c r="D181" t="s">
-        <v>188</v>
+        <v>265</v>
       </c>
       <c r="F181" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G181" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -3602,10 +3873,10 @@
         <v>5</v>
       </c>
       <c r="C183" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E183" t="s">
-        <v>188</v>
+        <v>266</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -3613,10 +3884,10 @@
         <v>5</v>
       </c>
       <c r="C184" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E184" t="s">
-        <v>188</v>
+        <v>266</v>
       </c>
     </row>
     <row r="185" spans="1:7">
@@ -3624,13 +3895,13 @@
         <v>8</v>
       </c>
       <c r="D185" t="s">
-        <v>188</v>
+        <v>266</v>
       </c>
       <c r="F185" t="s">
+        <v>246</v>
+      </c>
+      <c r="G185" t="s">
         <v>247</v>
-      </c>
-      <c r="G185" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="187" spans="1:7">
@@ -3638,10 +3909,10 @@
         <v>5</v>
       </c>
       <c r="C187" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E187" t="s">
-        <v>188</v>
+        <v>267</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -3649,10 +3920,10 @@
         <v>5</v>
       </c>
       <c r="C188" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E188" t="s">
-        <v>188</v>
+        <v>267</v>
       </c>
     </row>
     <row r="189" spans="1:7">
@@ -3660,265 +3931,266 @@
         <v>8</v>
       </c>
       <c r="D189" t="s">
-        <v>188</v>
+        <v>267</v>
       </c>
       <c r="F189" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G189" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A115:G158 A79:G81 A88:G94 A163:G187 A189:G1048576 A188:C188 E188:G188 A1:G77">
-    <cfRule type="expression" dxfId="65" priority="121">
+  <conditionalFormatting sqref="A115:G158 A79:G81 A88:G94 A188:C188 A1:G77 A163:G187 E188:G188 A189:G1048576">
+    <cfRule type="expression" dxfId="97" priority="121">
       <formula>$A1="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="122">
+    <cfRule type="expression" dxfId="96" priority="122">
       <formula>$A1="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88:G93">
-    <cfRule type="expression" dxfId="63" priority="59">
+    <cfRule type="expression" dxfId="95" priority="59">
       <formula>$A88="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="60">
+    <cfRule type="expression" dxfId="94" priority="60">
       <formula>$A88="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B157">
-    <cfRule type="expression" dxfId="61" priority="57">
+    <cfRule type="expression" dxfId="93" priority="57">
       <formula>$A157="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="58">
+    <cfRule type="expression" dxfId="92" priority="58">
       <formula>$A157="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A114:G114 A97:G97 A105:D110 F105:G110 A112:C113 E112:G113 A104:G104 A102:C103 E102:G103 A98:D101 F98:G101 A95:D95 F95:G95 A96:C96 E96:G96">
-    <cfRule type="expression" dxfId="59" priority="53">
+    <cfRule type="expression" dxfId="91" priority="53">
       <formula>$A95="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="54">
+    <cfRule type="expression" dxfId="90" priority="54">
       <formula>$A95="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A114:G114 A97:G97 A105:D110 F105:G110 A112:C113 E112:G113 A104:G104 A102:C103 E102:G103 A98:D101 F98:G101 A95:D95 F95:G95 A96:C96 E96:G96">
-    <cfRule type="expression" dxfId="57" priority="55">
+    <cfRule type="expression" dxfId="89" priority="55">
       <formula>$A95="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="56">
+    <cfRule type="expression" dxfId="88" priority="56">
       <formula>$A95="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A111:C111 E111:G111">
-    <cfRule type="expression" dxfId="55" priority="49">
+    <cfRule type="expression" dxfId="87" priority="49">
       <formula>$A111="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="50">
+    <cfRule type="expression" dxfId="86" priority="50">
       <formula>$A111="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A111:C111 E111:G111">
-    <cfRule type="expression" dxfId="53" priority="51">
+    <cfRule type="expression" dxfId="85" priority="51">
       <formula>$A111="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="52">
+    <cfRule type="expression" dxfId="84" priority="52">
       <formula>$A111="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A159:G162">
-    <cfRule type="expression" dxfId="51" priority="47">
+    <cfRule type="expression" dxfId="83" priority="47">
       <formula>$A159="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="48">
+    <cfRule type="expression" dxfId="82" priority="48">
       <formula>$A159="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E105">
-    <cfRule type="expression" dxfId="49" priority="45">
+    <cfRule type="expression" dxfId="81" priority="45">
       <formula>$A105="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="46">
+    <cfRule type="expression" dxfId="80" priority="46">
       <formula>$A105="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106">
-    <cfRule type="expression" dxfId="47" priority="43">
+    <cfRule type="expression" dxfId="79" priority="43">
       <formula>$A106="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="44">
+    <cfRule type="expression" dxfId="78" priority="44">
       <formula>$A106="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107">
-    <cfRule type="expression" dxfId="45" priority="41">
+    <cfRule type="expression" dxfId="77" priority="41">
       <formula>$A107="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="42">
+    <cfRule type="expression" dxfId="76" priority="42">
       <formula>$A107="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E108">
-    <cfRule type="expression" dxfId="43" priority="39">
+    <cfRule type="expression" dxfId="75" priority="39">
       <formula>$A108="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="40">
+    <cfRule type="expression" dxfId="74" priority="40">
       <formula>$A108="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109">
-    <cfRule type="expression" dxfId="41" priority="37">
+    <cfRule type="expression" dxfId="73" priority="37">
       <formula>$A109="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="38">
+    <cfRule type="expression" dxfId="72" priority="38">
       <formula>$A109="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E110">
-    <cfRule type="expression" dxfId="39" priority="35">
+    <cfRule type="expression" dxfId="71" priority="35">
       <formula>$A110="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="36">
+    <cfRule type="expression" dxfId="70" priority="36">
       <formula>$A110="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D111">
-    <cfRule type="expression" dxfId="37" priority="33">
+    <cfRule type="expression" dxfId="69" priority="33">
       <formula>$A111="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="34">
+    <cfRule type="expression" dxfId="68" priority="34">
       <formula>$A111="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D112">
-    <cfRule type="expression" dxfId="35" priority="31">
+    <cfRule type="expression" dxfId="67" priority="31">
       <formula>$A112="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="32">
+    <cfRule type="expression" dxfId="66" priority="32">
       <formula>$A112="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D113">
-    <cfRule type="expression" dxfId="33" priority="29">
+    <cfRule type="expression" dxfId="65" priority="29">
       <formula>$A113="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="30">
+    <cfRule type="expression" dxfId="64" priority="30">
       <formula>$A113="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="expression" dxfId="31" priority="27">
+    <cfRule type="expression" dxfId="63" priority="27">
       <formula>$A103="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="28">
+    <cfRule type="expression" dxfId="62" priority="28">
       <formula>$A103="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D102">
-    <cfRule type="expression" dxfId="29" priority="25">
+    <cfRule type="expression" dxfId="61" priority="25">
       <formula>$A102="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="26">
+    <cfRule type="expression" dxfId="60" priority="26">
       <formula>$A102="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E101">
-    <cfRule type="expression" dxfId="27" priority="23">
+    <cfRule type="expression" dxfId="59" priority="23">
       <formula>$A101="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="24">
+    <cfRule type="expression" dxfId="58" priority="24">
       <formula>$A101="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E100">
-    <cfRule type="expression" dxfId="25" priority="21">
+    <cfRule type="expression" dxfId="57" priority="21">
       <formula>$A100="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="22">
+    <cfRule type="expression" dxfId="56" priority="22">
       <formula>$A100="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E99">
-    <cfRule type="expression" dxfId="23" priority="19">
+    <cfRule type="expression" dxfId="55" priority="19">
       <formula>$A99="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="20">
+    <cfRule type="expression" dxfId="54" priority="20">
       <formula>$A99="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E98">
-    <cfRule type="expression" dxfId="21" priority="17">
+    <cfRule type="expression" dxfId="53" priority="17">
       <formula>$A98="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="18">
+    <cfRule type="expression" dxfId="52" priority="18">
       <formula>$A98="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E95">
-    <cfRule type="expression" dxfId="19" priority="15">
+    <cfRule type="expression" dxfId="51" priority="15">
       <formula>$A95="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="16">
+    <cfRule type="expression" dxfId="50" priority="16">
       <formula>$A95="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D96">
-    <cfRule type="expression" dxfId="17" priority="13">
+    <cfRule type="expression" dxfId="49" priority="13">
       <formula>$A96="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="48" priority="14">
       <formula>$A96="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78:G78">
-    <cfRule type="expression" dxfId="15" priority="11">
+    <cfRule type="expression" dxfId="47" priority="11">
       <formula>$A78="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="46" priority="12">
       <formula>$A78="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83:G83 A86:G87">
-    <cfRule type="expression" dxfId="13" priority="9">
+    <cfRule type="expression" dxfId="45" priority="9">
       <formula>$A83="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="10">
+    <cfRule type="expression" dxfId="44" priority="10">
       <formula>$A83="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:G82">
-    <cfRule type="expression" dxfId="11" priority="7">
+    <cfRule type="expression" dxfId="43" priority="7">
       <formula>$A82="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="42" priority="8">
       <formula>$A82="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:G85">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="41" priority="5">
       <formula>$A85="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="40" priority="6">
       <formula>$A85="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84:G84">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="39" priority="3">
       <formula>$A84="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="38" priority="4">
       <formula>$A84="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D188">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="37" priority="1">
       <formula>$A188="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="36" priority="2">
       <formula>$A188="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3948,16 +4220,16 @@
         <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3965,33 +4237,33 @@
         <v>117</v>
       </c>
       <c r="B2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" t="s">
         <v>203</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>204</v>
       </c>
-      <c r="D2" t="s">
-        <v>205</v>
-      </c>
       <c r="E2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3" t="s">
         <v>234</v>
       </c>
-      <c r="B3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D3" t="s">
-        <v>235</v>
-      </c>
       <c r="E3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3999,16 +4271,16 @@
         <v>119</v>
       </c>
       <c r="B4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" t="s">
         <v>237</v>
       </c>
-      <c r="C4" t="s">
-        <v>238</v>
-      </c>
       <c r="D4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -4018,10 +4290,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="35" priority="1">
       <formula>$A1="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="34" priority="2">
       <formula>$A1="Q"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4251,21 +4523,21 @@
         <v>117</v>
       </c>
       <c r="B35" t="s">
+        <v>202</v>
+      </c>
+      <c r="C35" t="s">
         <v>203</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>204</v>
-      </c>
-      <c r="D35" t="s">
-        <v>205</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F28">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="33" priority="1">
       <formula>$A1="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="32" priority="2">
       <formula>$A1="Q"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add Converstion Interaction base
</commit_message>
<xml_diff>
--- a/EmeraldAI/Data/TrainingData/DE_Training.xlsx
+++ b/EmeraldAI/Data/TrainingData/DE_Training.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="28860" windowHeight="17520"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="28860" windowHeight="17520" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sentence" sheetId="1" r:id="rId1"/>
     <sheet name="Action" sheetId="3" r:id="rId2"/>
-    <sheet name="Data" sheetId="2" r:id="rId3"/>
-    <sheet name="Interaction" sheetId="4" r:id="rId4"/>
+    <sheet name="Interaction" sheetId="4" r:id="rId3"/>
+    <sheet name="Data" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="285">
   <si>
     <t>Requirement</t>
   </si>
@@ -850,6 +850,36 @@
   </si>
   <si>
     <t>Sie sind {name}</t>
+  </si>
+  <si>
+    <t>Mache ein Update</t>
+  </si>
+  <si>
+    <t>Wann soll das Update durchgeführt werden?</t>
+  </si>
+  <si>
+    <t>An welchem Tag soll das Update durchgeführt werden?</t>
+  </si>
+  <si>
+    <t>Um welche Uhrzeit soll as Update durchgeführt werden?</t>
+  </si>
+  <si>
+    <t>Date:eqNone|Time:eqNone</t>
+  </si>
+  <si>
+    <t>Date:eqNone</t>
+  </si>
+  <si>
+    <t>Time:eqNone</t>
+  </si>
+  <si>
+    <t>Das Update wurde für den {date} um {time} geplant</t>
+  </si>
+  <si>
+    <t>Plane ein Update</t>
+  </si>
+  <si>
+    <t>ScheduleUpdate</t>
   </si>
 </sst>
 </file>
@@ -906,8 +936,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -999,7 +1041,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="99">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1043,6 +1085,12 @@
     <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1086,9 +1134,127 @@
     <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="120">
+  <dxfs count="136">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2207,9 +2373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
-    </sheetView>
+    <sheetView topLeftCell="A40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -4203,274 +4367,274 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A122:G165 A86:G88 A95:G101 A195:C195 A170:G194 E195:G195 A1:G47 A196:G1048576 A54:G84 C53:G53 A53">
-    <cfRule type="expression" dxfId="73" priority="125">
+    <cfRule type="expression" dxfId="75" priority="125">
       <formula>$A1="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="126">
+    <cfRule type="expression" dxfId="74" priority="126">
       <formula>$A1="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:G100">
-    <cfRule type="expression" dxfId="71" priority="63">
+    <cfRule type="expression" dxfId="73" priority="63">
       <formula>$A95="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="64">
+    <cfRule type="expression" dxfId="72" priority="64">
       <formula>$A95="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B164">
-    <cfRule type="expression" dxfId="69" priority="61">
+    <cfRule type="expression" dxfId="71" priority="61">
       <formula>$A164="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="62">
+    <cfRule type="expression" dxfId="70" priority="62">
       <formula>$A164="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A121:G121 A104:G104 A112:D117 F112:G117 A119:C120 E119:G120 A111:G111 A109:C110 E109:G110 A105:D108 F105:G108 A102:D102 F102:G102 A103:C103 E103:G103">
-    <cfRule type="expression" dxfId="67" priority="57">
+    <cfRule type="expression" dxfId="69" priority="57">
       <formula>$A102="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="58">
+    <cfRule type="expression" dxfId="68" priority="58">
       <formula>$A102="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A121:G121 A104:G104 A112:D117 F112:G117 A119:C120 E119:G120 A111:G111 A109:C110 E109:G110 A105:D108 F105:G108 A102:D102 F102:G102 A103:C103 E103:G103">
-    <cfRule type="expression" dxfId="65" priority="59">
+    <cfRule type="expression" dxfId="67" priority="59">
       <formula>$A102="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="60">
+    <cfRule type="expression" dxfId="66" priority="60">
       <formula>$A102="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A118:C118 E118:G118">
-    <cfRule type="expression" dxfId="63" priority="53">
+    <cfRule type="expression" dxfId="65" priority="53">
       <formula>$A118="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="54">
+    <cfRule type="expression" dxfId="64" priority="54">
       <formula>$A118="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A118:C118 E118:G118">
-    <cfRule type="expression" dxfId="61" priority="55">
+    <cfRule type="expression" dxfId="63" priority="55">
       <formula>$A118="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="56">
+    <cfRule type="expression" dxfId="62" priority="56">
       <formula>$A118="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A166:G169">
-    <cfRule type="expression" dxfId="59" priority="51">
+    <cfRule type="expression" dxfId="61" priority="51">
       <formula>$A166="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="52">
+    <cfRule type="expression" dxfId="60" priority="52">
       <formula>$A166="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E112">
-    <cfRule type="expression" dxfId="57" priority="49">
+    <cfRule type="expression" dxfId="59" priority="49">
       <formula>$A112="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="50">
+    <cfRule type="expression" dxfId="58" priority="50">
       <formula>$A112="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E113">
-    <cfRule type="expression" dxfId="55" priority="47">
+    <cfRule type="expression" dxfId="57" priority="47">
       <formula>$A113="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="48">
+    <cfRule type="expression" dxfId="56" priority="48">
       <formula>$A113="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E114">
-    <cfRule type="expression" dxfId="53" priority="45">
+    <cfRule type="expression" dxfId="55" priority="45">
       <formula>$A114="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="46">
+    <cfRule type="expression" dxfId="54" priority="46">
       <formula>$A114="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E115">
-    <cfRule type="expression" dxfId="51" priority="43">
+    <cfRule type="expression" dxfId="53" priority="43">
       <formula>$A115="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="44">
+    <cfRule type="expression" dxfId="52" priority="44">
       <formula>$A115="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E116">
-    <cfRule type="expression" dxfId="49" priority="41">
+    <cfRule type="expression" dxfId="51" priority="41">
       <formula>$A116="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="42">
+    <cfRule type="expression" dxfId="50" priority="42">
       <formula>$A116="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E117">
-    <cfRule type="expression" dxfId="47" priority="39">
+    <cfRule type="expression" dxfId="49" priority="39">
       <formula>$A117="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="40">
+    <cfRule type="expression" dxfId="48" priority="40">
       <formula>$A117="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D118">
-    <cfRule type="expression" dxfId="45" priority="37">
+    <cfRule type="expression" dxfId="47" priority="37">
       <formula>$A118="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="38">
+    <cfRule type="expression" dxfId="46" priority="38">
       <formula>$A118="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D119">
-    <cfRule type="expression" dxfId="43" priority="35">
+    <cfRule type="expression" dxfId="45" priority="35">
       <formula>$A119="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="36">
+    <cfRule type="expression" dxfId="44" priority="36">
       <formula>$A119="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D120">
-    <cfRule type="expression" dxfId="41" priority="33">
+    <cfRule type="expression" dxfId="43" priority="33">
       <formula>$A120="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="34">
+    <cfRule type="expression" dxfId="42" priority="34">
       <formula>$A120="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110">
-    <cfRule type="expression" dxfId="39" priority="31">
+    <cfRule type="expression" dxfId="41" priority="31">
       <formula>$A110="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="32">
+    <cfRule type="expression" dxfId="40" priority="32">
       <formula>$A110="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D109">
-    <cfRule type="expression" dxfId="37" priority="29">
+    <cfRule type="expression" dxfId="39" priority="29">
       <formula>$A109="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="30">
+    <cfRule type="expression" dxfId="38" priority="30">
       <formula>$A109="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E108">
-    <cfRule type="expression" dxfId="35" priority="27">
+    <cfRule type="expression" dxfId="37" priority="27">
       <formula>$A108="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="28">
+    <cfRule type="expression" dxfId="36" priority="28">
       <formula>$A108="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107">
-    <cfRule type="expression" dxfId="33" priority="25">
+    <cfRule type="expression" dxfId="35" priority="25">
       <formula>$A107="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="26">
+    <cfRule type="expression" dxfId="34" priority="26">
       <formula>$A107="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106">
-    <cfRule type="expression" dxfId="31" priority="23">
+    <cfRule type="expression" dxfId="33" priority="23">
       <formula>$A106="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="24">
+    <cfRule type="expression" dxfId="32" priority="24">
       <formula>$A106="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E105">
-    <cfRule type="expression" dxfId="29" priority="21">
+    <cfRule type="expression" dxfId="31" priority="21">
       <formula>$A105="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="22">
+    <cfRule type="expression" dxfId="30" priority="22">
       <formula>$A105="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E102">
-    <cfRule type="expression" dxfId="27" priority="19">
+    <cfRule type="expression" dxfId="29" priority="19">
       <formula>$A102="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="20">
+    <cfRule type="expression" dxfId="28" priority="20">
       <formula>$A102="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103">
-    <cfRule type="expression" dxfId="25" priority="17">
+    <cfRule type="expression" dxfId="27" priority="17">
       <formula>$A103="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="18">
+    <cfRule type="expression" dxfId="26" priority="18">
       <formula>$A103="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:G85">
-    <cfRule type="expression" dxfId="23" priority="15">
+    <cfRule type="expression" dxfId="25" priority="15">
       <formula>$A85="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="16">
+    <cfRule type="expression" dxfId="24" priority="16">
       <formula>$A85="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90:G90 A93:G94">
-    <cfRule type="expression" dxfId="21" priority="13">
+    <cfRule type="expression" dxfId="23" priority="13">
       <formula>$A90="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="14">
+    <cfRule type="expression" dxfId="22" priority="14">
       <formula>$A90="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A89:G89">
-    <cfRule type="expression" dxfId="19" priority="11">
+    <cfRule type="expression" dxfId="21" priority="11">
       <formula>$A89="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="12">
+    <cfRule type="expression" dxfId="20" priority="12">
       <formula>$A89="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A92:G92">
-    <cfRule type="expression" dxfId="17" priority="9">
+    <cfRule type="expression" dxfId="19" priority="9">
       <formula>$A92="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="10">
+    <cfRule type="expression" dxfId="18" priority="10">
       <formula>$A92="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91:G91">
-    <cfRule type="expression" dxfId="15" priority="7">
+    <cfRule type="expression" dxfId="17" priority="7">
       <formula>$A91="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="8">
+    <cfRule type="expression" dxfId="16" priority="8">
       <formula>$A91="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D195">
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>$A195="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>$A195="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:G51 A52 C52:G52">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>$A48="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>$A48="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="expression" dxfId="5" priority="131">
+    <cfRule type="expression" dxfId="11" priority="131">
       <formula>$A53="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="132">
+    <cfRule type="expression" dxfId="10" priority="132">
       <formula>$A53="Q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>$A53="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>$A53="Q"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4575,10 +4739,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$A1="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$A1="Q"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4593,10 +4757,136 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="7.1640625" customWidth="1"/>
+    <col min="2" max="2" width="39.5" customWidth="1"/>
+    <col min="3" max="3" width="97.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>280</v>
+      </c>
+      <c r="C5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C6" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>282</v>
+      </c>
+      <c r="E7" t="s">
+        <v>284</v>
+      </c>
+      <c r="F7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:F1000">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>$A1="A"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>$A1="Q"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4819,10 +5109,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:F28">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$A1="A"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A1="Q"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4833,21 +5123,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix not equal indicator
</commit_message>
<xml_diff>
--- a/EmeraldAI/Data/TrainingData/DE_Training.xlsx
+++ b/EmeraldAI/Data/TrainingData/DE_Training.xlsx
@@ -888,7 +888,7 @@
     <t>ScheduleUpdateDate:eqNone</t>
   </si>
   <si>
-    <t>ScheduleUpdateDate:neqNone|ScheduleUpdateTime:neqNone</t>
+    <t>ScheduleUpdateDate:neNone|ScheduleUpdateTime:neNone</t>
   </si>
 </sst>
 </file>
@@ -2102,7 +2102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G196"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A60" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -4488,7 +4488,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>